<commit_message>
Deploying to gh-pages from @ AlvaroGohe/AlvaroGohe.github.io@d149c2b845cceda4d52ee354c0b9d04702064193 🚀
</commit_message>
<xml_diff>
--- a/Conferences.xlsx
+++ b/Conferences.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -129,6 +129,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -138,14 +139,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -155,14 +158,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of January, 2024</t>
     </r>
@@ -191,6 +196,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14</t>
     </r>
@@ -200,14 +206,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 15</t>
     </r>
@@ -217,14 +225,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -250,6 +260,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
     </r>
@@ -259,14 +270,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 8</t>
     </r>
@@ -276,14 +289,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -303,6 +318,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -312,14 +328,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of August - 1</t>
     </r>
@@ -329,6 +347,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -337,6 +356,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -356,6 +376,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">27</t>
     </r>
@@ -365,14 +386,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 31</t>
     </r>
@@ -382,6 +405,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -390,6 +414,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of March, 2023</t>
     </r>
@@ -418,6 +443,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -427,14 +453,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of May - 2</t>
     </r>
@@ -444,6 +472,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -452,6 +481,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2023</t>
     </r>
@@ -501,6 +531,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -510,6 +541,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -518,6 +550,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 6</t>
     </r>
@@ -527,14 +560,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of May, 2023</t>
     </r>
@@ -554,6 +589,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -563,14 +599,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 7</t>
     </r>
@@ -580,14 +618,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of April, 2022</t>
     </r>
@@ -619,6 +659,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -628,14 +669,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -645,14 +688,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of July, 2024</t>
     </r>
@@ -672,6 +717,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">17</t>
     </r>
@@ -681,14 +727,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 21</t>
     </r>
@@ -698,6 +746,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -706,6 +755,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2024</t>
     </r>
@@ -746,6 +796,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">22</t>
     </r>
@@ -755,6 +806,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -763,6 +815,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 27</t>
     </r>
@@ -772,14 +825,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of July, 2019</t>
     </r>
@@ -811,6 +866,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">24</t>
     </r>
@@ -820,14 +876,16 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  - 29</t>
     </r>
@@ -837,20 +895,34 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of July, 2023</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">https://enem.anem.es/2023/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Durham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference of the UK Algebraic Geometry Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11th - 12th September, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ukagnetwork.org/upcoming-activities/durham-september-2024</t>
   </si>
 </sst>
 </file>
@@ -865,6 +937,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -886,12 +959,14 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -962,13 +1037,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.24"/>
@@ -1474,6 +1549,26 @@
         <v>112</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>-1.57217905973651</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>54.7638082226076</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://y-rant.github.io/"/>
@@ -1491,6 +1586,7 @@
     <hyperlink ref="F15" r:id="rId13" display="http://emiliano.ambrosi.perso.math.cnrs.fr/CAVARETpage/Cavaretmain.html"/>
     <hyperlink ref="F18" r:id="rId14" display="https://www.icmat.es/es/actividades/escuela-jae/programa2019/"/>
     <hyperlink ref="F19" r:id="rId15" display="https://enem.anem.es/2023/"/>
+    <hyperlink ref="F20" r:id="rId16" display="https://www.ukagnetwork.org/upcoming-activities/durham-september-2024"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added outreach talks, announcements, fixed minor mistakes
</commit_message>
<xml_diff>
--- a/Conferences.xlsx
+++ b/Conferences.xlsx
@@ -129,7 +129,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -139,16 +138,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -158,16 +155,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of January, 2024</t>
     </r>
@@ -196,7 +191,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14</t>
     </r>
@@ -206,16 +200,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 15</t>
     </r>
@@ -225,16 +217,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -260,7 +250,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
     </r>
@@ -270,16 +259,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 8</t>
     </r>
@@ -289,16 +276,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -318,7 +303,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -328,16 +312,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of August - 1</t>
     </r>
@@ -347,7 +329,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -356,7 +337,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -376,7 +356,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">27</t>
     </r>
@@ -386,16 +365,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 31</t>
     </r>
@@ -405,7 +382,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -414,7 +390,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of March, 2023</t>
     </r>
@@ -443,7 +418,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -453,16 +427,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of May - 2</t>
     </r>
@@ -472,7 +444,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -481,7 +452,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2023</t>
     </r>
@@ -531,7 +501,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -541,7 +510,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -550,7 +518,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 6</t>
     </r>
@@ -560,16 +527,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of May, 2023</t>
     </r>
@@ -589,7 +554,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -599,16 +563,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 7</t>
     </r>
@@ -618,16 +580,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of April, 2022</t>
     </r>
@@ -659,7 +619,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -669,16 +628,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -688,16 +645,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2024</t>
     </r>
@@ -717,7 +672,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">17</t>
     </r>
@@ -727,16 +681,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 21</t>
     </r>
@@ -746,7 +698,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -755,7 +706,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2024</t>
     </r>
@@ -796,7 +746,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">22</t>
     </r>
@@ -806,7 +755,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -815,7 +763,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 27</t>
     </r>
@@ -825,16 +772,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2019</t>
     </r>
@@ -866,7 +811,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">24</t>
     </r>
@@ -876,16 +820,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  - 29</t>
     </r>
@@ -895,16 +837,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2023</t>
     </r>
@@ -937,7 +877,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -959,14 +898,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1037,14 +974,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="A29:B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.28"/>
@@ -1053,12 +991,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="60.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="19" style="0" width="15.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,7 +1099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>-5.98730327116186</v>
       </c>
@@ -1195,7 +1137,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>-1.19228572883472</v>
       </c>
@@ -1224,7 +1166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.102929620693971</v>
       </c>
@@ -1253,7 +1195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.726789018276719</v>
       </c>
@@ -1273,7 +1215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>-1.55975565552009</v>
       </c>
@@ -1302,7 +1244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>4.45803780961967</v>
       </c>
@@ -1360,7 +1302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>12.4902540508099</v>
       </c>
@@ -1380,7 +1322,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>-1.93047013602202</v>
       </c>
@@ -1420,7 +1362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>-3.70834181894173</v>
       </c>
@@ -1440,7 +1382,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>2.16373781349128</v>
       </c>
@@ -1489,7 +1431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>-3.60933080558135</v>
       </c>
@@ -1529,7 +1471,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>-7.00757048938887</v>
       </c>
@@ -1567,6 +1509,12 @@
       </c>
       <c r="F20" s="1" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <f aca="false">AVERAGE(A2:A28)</f>
+        <v>-6.18893032235353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ AlvaroGohe/AlvaroGohe.github.io@d254f06320283f7122659d7932ad4d48b2a20637 🚀
</commit_message>
<xml_diff>
--- a/Conferences.xlsx
+++ b/Conferences.xlsx
@@ -129,7 +129,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -139,16 +138,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -158,16 +155,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of January, 2024</t>
     </r>
@@ -196,7 +191,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14</t>
     </r>
@@ -206,16 +200,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 15</t>
     </r>
@@ -225,16 +217,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -260,7 +250,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
     </r>
@@ -270,16 +259,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 8</t>
     </r>
@@ -289,16 +276,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -318,7 +303,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -328,16 +312,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of August - 1</t>
     </r>
@@ -347,7 +329,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -356,7 +337,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of September, 2023</t>
     </r>
@@ -376,7 +356,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">27</t>
     </r>
@@ -386,16 +365,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 31</t>
     </r>
@@ -405,7 +382,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -414,7 +390,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of March, 2023</t>
     </r>
@@ -443,7 +418,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30</t>
     </r>
@@ -453,16 +427,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of May - 2</t>
     </r>
@@ -472,7 +444,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -481,7 +452,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2023</t>
     </r>
@@ -531,7 +501,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -541,7 +510,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -550,7 +518,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 6</t>
     </r>
@@ -560,16 +527,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of May, 2023</t>
     </r>
@@ -589,7 +554,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -599,16 +563,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 7</t>
     </r>
@@ -618,16 +580,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of April, 2022</t>
     </r>
@@ -659,7 +619,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
     </r>
@@ -669,16 +628,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 12</t>
     </r>
@@ -688,16 +645,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2024</t>
     </r>
@@ -717,7 +672,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">17</t>
     </r>
@@ -727,16 +681,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 21</t>
     </r>
@@ -746,7 +698,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -755,7 +706,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> of June, 2024</t>
     </r>
@@ -796,7 +746,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">22</t>
     </r>
@@ -806,7 +755,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -815,7 +763,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> - 27</t>
     </r>
@@ -825,16 +772,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2019</t>
     </r>
@@ -866,7 +811,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">24</t>
     </r>
@@ -876,16 +820,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  - 29</t>
     </r>
@@ -895,16 +837,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">th</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of July, 2023</t>
     </r>
@@ -937,7 +877,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -959,14 +898,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1037,14 +974,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="A29:B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.28"/>
@@ -1053,12 +991,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="60.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="19" style="0" width="15.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,7 +1099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>-5.98730327116186</v>
       </c>
@@ -1195,7 +1137,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>-1.19228572883472</v>
       </c>
@@ -1224,7 +1166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0.102929620693971</v>
       </c>
@@ -1253,7 +1195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.726789018276719</v>
       </c>
@@ -1273,7 +1215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>-1.55975565552009</v>
       </c>
@@ -1302,7 +1244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>4.45803780961967</v>
       </c>
@@ -1360,7 +1302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>12.4902540508099</v>
       </c>
@@ -1380,7 +1322,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>-1.93047013602202</v>
       </c>
@@ -1420,7 +1362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>-3.70834181894173</v>
       </c>
@@ -1440,7 +1382,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>2.16373781349128</v>
       </c>
@@ -1489,7 +1431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>-3.60933080558135</v>
       </c>
@@ -1529,7 +1471,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>-7.00757048938887</v>
       </c>
@@ -1567,6 +1509,12 @@
       </c>
       <c r="F20" s="1" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <f aca="false">AVERAGE(A2:A28)</f>
+        <v>-6.18893032235353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>